<commit_message>
main.c modifications, changed interupts and some other stuff.
</commit_message>
<xml_diff>
--- a/Project/Mech 458 Project Wiring.xlsx
+++ b/Project/Mech 458 Project Wiring.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benne\GitHub\Mech458\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4537e0bdef8c4a1e/Documents/GitHub/Mech458/Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05E040BA-F6BE-4530-9EE3-9833FA32FDD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{05E040BA-F6BE-4530-9EE3-9833FA32FDD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F697576E-FF66-467F-9DAB-C289CA9D887A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6DB3E047-77CC-4596-8068-2C12ABE17B1D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6DB3E047-77CC-4596-8068-2C12ABE17B1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -451,12 +451,6 @@
   <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -478,17 +472,11 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -498,7 +486,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -512,6 +500,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -867,21 +867,21 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="64.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="64.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -900,380 +900,380 @@
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="15" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="2">
         <v>3</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="2">
         <v>27</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="5" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="25"/>
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="3">
         <v>4</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="3">
         <v>26</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="25"/>
+      <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="2">
         <v>5</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="2">
         <v>25</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="5" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="25"/>
+      <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="3">
         <v>6</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="3">
         <v>24</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="25"/>
+      <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="2">
         <v>7</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="2">
         <v>23</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="5" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="25"/>
+      <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="3">
         <v>8</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="3">
         <v>22</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="14"/>
-      <c r="B9" s="8" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="26"/>
+      <c r="B9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="6">
         <v>23</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="14"/>
-      <c r="B10" s="7" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="26"/>
+      <c r="B10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="11"/>
-      <c r="B12" s="13" t="s">
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="27"/>
+      <c r="B12" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="11"/>
-      <c r="B13" s="12" t="s">
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="27"/>
+      <c r="B13" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="12">
+      <c r="D13" s="9">
         <v>23</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G13" s="23" t="s">
+      <c r="G13" s="19" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="11"/>
-      <c r="B14" s="13" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="27"/>
+      <c r="B14" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14" s="10">
         <v>20</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="10">
         <v>3</v>
       </c>
-      <c r="F14" s="22" t="s">
+      <c r="F14" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="G14" s="22" t="s">
+      <c r="G14" s="18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="11"/>
-      <c r="B15" s="12" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="27"/>
+      <c r="B15" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="11"/>
-      <c r="B16" s="13" t="s">
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="27"/>
+      <c r="B16" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="16">
+      <c r="D17" s="12">
         <v>32</v>
       </c>
-      <c r="E17" s="16">
+      <c r="E17" s="12">
         <v>53</v>
       </c>
-      <c r="F17" s="21" t="s">
+      <c r="F17" s="17" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
-      <c r="B18" s="17" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="28"/>
+      <c r="B18" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-      <c r="B19" s="15" t="s">
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="28"/>
+      <c r="B19" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-      <c r="B20" s="17" t="s">
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="28"/>
+      <c r="B20" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="18">
+      <c r="D20" s="14">
         <v>31</v>
       </c>
-      <c r="E20" s="18">
+      <c r="E20" s="14">
         <v>52</v>
       </c>
-      <c r="F20" s="20" t="s">
+      <c r="F20" s="16" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-      <c r="B21" s="15" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="28"/>
+      <c r="B21" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="21" t="s">
+      <c r="C21" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="16">
+      <c r="D21" s="12">
         <v>26</v>
       </c>
-      <c r="E21" s="16">
+      <c r="E21" s="12">
         <v>13</v>
       </c>
-      <c r="F21" s="16"/>
-    </row>
-    <row r="24" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F21" s="12"/>
+    </row>
+    <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
         <v>48</v>
       </c>
       <c r="B25" s="30"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="25" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="24">
+      <c r="B26" s="20">
         <v>455</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="25" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="26">
+      <c r="B27" s="22">
         <v>445</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="25" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="26">
+      <c r="B28" s="22">
         <v>435</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="25" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B29" s="26"/>
-    </row>
-    <row r="30" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="27" t="s">
+      <c r="B29" s="22"/>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="B30" s="28"/>
+      <c r="B30" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
Created ISR Routine to pause program and Updated Excel Pin Sheet
</commit_message>
<xml_diff>
--- a/Project/Mech 458 Project Wiring.xlsx
+++ b/Project/Mech 458 Project Wiring.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4537e0bdef8c4a1e/Documents/GitHub/Mech458/Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benne\GitHub\Mech458\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{05E040BA-F6BE-4530-9EE3-9833FA32FDD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F697576E-FF66-467F-9DAB-C289CA9D887A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89467C6F-45E7-44DC-890E-E3748705C6B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6DB3E047-77CC-4596-8068-2C12ABE17B1D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6DB3E047-77CC-4596-8068-2C12ABE17B1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="63">
   <si>
     <t>Breadboard Pin</t>
   </si>
@@ -198,6 +198,33 @@
   </si>
   <si>
     <t>Rest</t>
+  </si>
+  <si>
+    <t>Buttons</t>
+  </si>
+  <si>
+    <t>Pause button</t>
+  </si>
+  <si>
+    <t>F-J</t>
+  </si>
+  <si>
+    <t>INT2 and PORTD:2</t>
+  </si>
+  <si>
+    <t>End button</t>
+  </si>
+  <si>
+    <t>INT1 and PORTD:1</t>
+  </si>
+  <si>
+    <t>Button is normally low</t>
+  </si>
+  <si>
+    <t>INT0 and PORTD:0</t>
+  </si>
+  <si>
+    <t>Optical Sensor For Bucket, Normally Low</t>
   </si>
 </sst>
 </file>
@@ -227,7 +254,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -302,8 +329,25 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -432,8 +476,67 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -447,8 +550,11 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
@@ -518,20 +624,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="10" xfId="13" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="11" xfId="13" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="12" xfId="15" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="12" xfId="15" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="13" xfId="15" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="14" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="14" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="14" xfId="14" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="16">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
     <cellStyle name="20% - Accent2" xfId="5" builtinId="34"/>
     <cellStyle name="20% - Accent3" xfId="8" builtinId="38"/>
     <cellStyle name="20% - Accent5" xfId="11" builtinId="46"/>
+    <cellStyle name="40% - Accent6" xfId="14" builtinId="51"/>
     <cellStyle name="60% - Accent1" xfId="3" builtinId="32"/>
     <cellStyle name="60% - Accent2" xfId="6" builtinId="36"/>
     <cellStyle name="60% - Accent3" xfId="9" builtinId="40"/>
     <cellStyle name="60% - Accent5" xfId="12" builtinId="48"/>
+    <cellStyle name="60% - Accent6" xfId="15" builtinId="52"/>
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
     <cellStyle name="Accent2" xfId="4" builtinId="33"/>
     <cellStyle name="Accent3" xfId="7" builtinId="37"/>
     <cellStyle name="Accent5" xfId="10" builtinId="45"/>
+    <cellStyle name="Accent6" xfId="13" builtinId="49"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -867,21 +992,21 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="64.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="64.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -904,7 +1029,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
         <v>4</v>
       </c>
@@ -924,7 +1049,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="25"/>
       <c r="B3" s="3" t="s">
         <v>7</v>
@@ -942,7 +1067,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="25"/>
       <c r="B4" s="2" t="s">
         <v>8</v>
@@ -960,7 +1085,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="25"/>
       <c r="B5" s="3" t="s">
         <v>9</v>
@@ -978,7 +1103,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="25"/>
       <c r="B6" s="2" t="s">
         <v>10</v>
@@ -996,7 +1121,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="25"/>
       <c r="B7" s="3" t="s">
         <v>11</v>
@@ -1014,7 +1139,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="26" t="s">
         <v>20</v>
       </c>
@@ -1034,7 +1159,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="26"/>
       <c r="B9" s="6" t="s">
         <v>22</v>
@@ -1052,7 +1177,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="26"/>
       <c r="B10" s="5" t="s">
         <v>23</v>
@@ -1070,7 +1195,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="27" t="s">
         <v>30</v>
       </c>
@@ -1082,17 +1207,28 @@
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="27"/>
       <c r="B12" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C12" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="10">
+        <v>21</v>
+      </c>
+      <c r="E12" s="10">
+        <v>21</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" s="18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="27"/>
       <c r="B13" s="9" t="s">
         <v>33</v>
@@ -1113,7 +1249,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="27"/>
       <c r="B14" s="10" t="s">
         <v>34</v>
@@ -1134,7 +1270,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="27"/>
       <c r="B15" s="9" t="s">
         <v>35</v>
@@ -1144,7 +1280,7 @@
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="27"/>
       <c r="B16" s="10" t="s">
         <v>36</v>
@@ -1154,7 +1290,7 @@
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="28" t="s">
         <v>29</v>
       </c>
@@ -1174,7 +1310,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="28"/>
       <c r="B18" s="13" t="s">
         <v>38</v>
@@ -1186,7 +1322,7 @@
       <c r="E18" s="14"/>
       <c r="F18" s="14"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="28"/>
       <c r="B19" s="11" t="s">
         <v>39</v>
@@ -1198,7 +1334,7 @@
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="28"/>
       <c r="B20" s="13" t="s">
         <v>40</v>
@@ -1216,7 +1352,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="28"/>
       <c r="B21" s="11" t="s">
         <v>41</v>
@@ -1232,14 +1368,58 @@
       </c>
       <c r="F21" s="12"/>
     </row>
-    <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="37">
+        <v>54</v>
+      </c>
+      <c r="E22" s="37">
+        <v>20</v>
+      </c>
+      <c r="F22" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="G22" s="37" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="32"/>
+      <c r="B23" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="34">
+        <v>51</v>
+      </c>
+      <c r="E23" s="34">
+        <v>19</v>
+      </c>
+      <c r="F23" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="G23" s="34" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="29" t="s">
         <v>48</v>
       </c>
       <c r="B25" s="30"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="21" t="s">
         <v>53</v>
       </c>
@@ -1247,7 +1427,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="21" t="s">
         <v>49</v>
       </c>
@@ -1255,7 +1435,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="21" t="s">
         <v>50</v>
       </c>
@@ -1263,25 +1443,26 @@
         <v>435</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="21" t="s">
         <v>51</v>
       </c>
       <c r="B29" s="22"/>
     </row>
-    <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="23" t="s">
         <v>52</v>
       </c>
       <c r="B30" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="A11:A16"/>
     <mergeCell ref="A17:A21"/>
     <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A22:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Got a delay timer working to give items time to drop into tray before moving it.
</commit_message>
<xml_diff>
--- a/Project/Mech 458 Project Wiring.xlsx
+++ b/Project/Mech 458 Project Wiring.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benne\GitHub\Mech458\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C209491-C92C-46ED-9B00-5AEC7F14FD24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13650C10-2324-4D56-9CB5-FE885F1572C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{6DB3E047-77CC-4596-8068-2C12ABE17B1D}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{6DB3E047-77CC-4596-8068-2C12ABE17B1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="69">
   <si>
     <t>Breadboard Pin</t>
   </si>
@@ -243,15 +243,6 @@
   </si>
   <si>
     <t>500&lt;x&lt;600</t>
-  </si>
-  <si>
-    <t>29/30</t>
-  </si>
-  <si>
-    <t>50/51</t>
-  </si>
-  <si>
-    <t>PORTB:2 or 3</t>
   </si>
 </sst>
 </file>
@@ -647,6 +638,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -670,12 +667,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="11" xfId="13" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="16">
@@ -1030,7 +1021,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17:A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1068,7 +1059,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="33" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1088,7 +1079,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="31"/>
+      <c r="A3" s="33"/>
       <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
@@ -1106,7 +1097,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="31"/>
+      <c r="A4" s="33"/>
       <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1124,7 +1115,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="31"/>
+      <c r="A5" s="33"/>
       <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
@@ -1142,7 +1133,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="31"/>
+      <c r="A6" s="33"/>
       <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1160,7 +1151,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="31"/>
+      <c r="A7" s="33"/>
       <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
@@ -1178,7 +1169,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="34" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -1198,7 +1189,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="32"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="6" t="s">
         <v>22</v>
       </c>
@@ -1216,7 +1207,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="32"/>
+      <c r="A10" s="34"/>
       <c r="B10" s="5" t="s">
         <v>23</v>
       </c>
@@ -1234,7 +1225,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="35" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -1254,7 +1245,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="33"/>
+      <c r="A12" s="35"/>
       <c r="B12" s="10" t="s">
         <v>32</v>
       </c>
@@ -1275,7 +1266,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="33"/>
+      <c r="A13" s="35"/>
       <c r="B13" s="9" t="s">
         <v>33</v>
       </c>
@@ -1296,7 +1287,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="33"/>
+      <c r="A14" s="35"/>
       <c r="B14" s="10" t="s">
         <v>34</v>
       </c>
@@ -1317,7 +1308,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="33"/>
+      <c r="A15" s="35"/>
       <c r="B15" s="9" t="s">
         <v>35</v>
       </c>
@@ -1327,7 +1318,7 @@
       <c r="F15" s="9"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="33"/>
+      <c r="A16" s="35"/>
       <c r="B16" s="10" t="s">
         <v>36</v>
       </c>
@@ -1337,7 +1328,7 @@
       <c r="F16" s="10"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="36" t="s">
         <v>29</v>
       </c>
       <c r="B17" s="11" t="s">
@@ -1357,43 +1348,35 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="34"/>
+      <c r="A18" s="36"/>
       <c r="B18" s="13" t="s">
         <v>38</v>
       </c>
       <c r="C18" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="E18" s="39" t="s">
-        <v>70</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>71</v>
-      </c>
+      <c r="D18" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="31"/>
+      <c r="F18" s="14"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="34"/>
+      <c r="A19" s="36"/>
       <c r="B19" s="11" t="s">
         <v>39</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="40" t="s">
-        <v>69</v>
-      </c>
-      <c r="E19" s="40" t="s">
-        <v>70</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>71</v>
-      </c>
+      <c r="D19" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="32"/>
+      <c r="F19" s="12"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="34"/>
+      <c r="A20" s="36"/>
       <c r="B20" s="13" t="s">
         <v>40</v>
       </c>
@@ -1403,7 +1386,7 @@
       <c r="D20" s="14">
         <v>31</v>
       </c>
-      <c r="E20" s="39">
+      <c r="E20" s="31">
         <v>52</v>
       </c>
       <c r="F20" s="16" t="s">
@@ -1411,7 +1394,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="34"/>
+      <c r="A21" s="36"/>
       <c r="B21" s="11" t="s">
         <v>41</v>
       </c>
@@ -1427,7 +1410,7 @@
       <c r="F21" s="12"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="37" t="s">
+      <c r="A22" s="39" t="s">
         <v>54</v>
       </c>
       <c r="B22" s="26" t="s">
@@ -1450,7 +1433,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="38"/>
+      <c r="A23" s="40"/>
       <c r="B23" s="23" t="s">
         <v>55</v>
       </c>
@@ -1472,10 +1455,10 @@
     </row>
     <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="35" t="s">
+      <c r="A25" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="36"/>
+      <c r="B25" s="38"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="21" t="s">

</xml_diff>

<commit_message>
Probably the last push
</commit_message>
<xml_diff>
--- a/Project/Mech 458 Project Wiring.xlsx
+++ b/Project/Mech 458 Project Wiring.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benne\GitHub\Mech458\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4537e0bdef8c4a1e/Documents/GitHub/Mech458/Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13650C10-2324-4D56-9CB5-FE885F1572C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{13650C10-2324-4D56-9CB5-FE885F1572C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{146F7878-8ED3-4492-B028-4CCEE266EAD4}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{6DB3E047-77CC-4596-8068-2C12ABE17B1D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6DB3E047-77CC-4596-8068-2C12ABE17B1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1021,21 +1021,21 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17:A21"/>
+      <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="64.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="64.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1058,7 +1058,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>4</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="33"/>
       <c r="B3" s="3" t="s">
         <v>7</v>
@@ -1096,7 +1096,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="33"/>
       <c r="B4" s="2" t="s">
         <v>8</v>
@@ -1114,7 +1114,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="33"/>
       <c r="B5" s="3" t="s">
         <v>9</v>
@@ -1132,7 +1132,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="33"/>
       <c r="B6" s="2" t="s">
         <v>10</v>
@@ -1150,7 +1150,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="33"/>
       <c r="B7" s="3" t="s">
         <v>11</v>
@@ -1168,7 +1168,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="34" t="s">
         <v>20</v>
       </c>
@@ -1188,7 +1188,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="34"/>
       <c r="B9" s="6" t="s">
         <v>22</v>
@@ -1206,7 +1206,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="34"/>
       <c r="B10" s="5" t="s">
         <v>23</v>
@@ -1224,7 +1224,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="35" t="s">
         <v>30</v>
       </c>
@@ -1244,7 +1244,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="35"/>
       <c r="B12" s="10" t="s">
         <v>32</v>
@@ -1265,7 +1265,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="35"/>
       <c r="B13" s="9" t="s">
         <v>33</v>
@@ -1286,7 +1286,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="35"/>
       <c r="B14" s="10" t="s">
         <v>34</v>
@@ -1307,7 +1307,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="35"/>
       <c r="B15" s="9" t="s">
         <v>35</v>
@@ -1317,7 +1317,7 @@
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="35"/>
       <c r="B16" s="10" t="s">
         <v>36</v>
@@ -1327,7 +1327,7 @@
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="36" t="s">
         <v>29</v>
       </c>
@@ -1347,7 +1347,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="36"/>
       <c r="B18" s="13" t="s">
         <v>38</v>
@@ -1361,7 +1361,7 @@
       <c r="E18" s="31"/>
       <c r="F18" s="14"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="36"/>
       <c r="B19" s="11" t="s">
         <v>39</v>
@@ -1375,7 +1375,7 @@
       <c r="E19" s="32"/>
       <c r="F19" s="12"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="36"/>
       <c r="B20" s="13" t="s">
         <v>40</v>
@@ -1393,7 +1393,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="36"/>
       <c r="B21" s="11" t="s">
         <v>41</v>
@@ -1409,7 +1409,7 @@
       </c>
       <c r="F21" s="12"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="39" t="s">
         <v>54</v>
       </c>
@@ -1432,7 +1432,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="40"/>
       <c r="B23" s="23" t="s">
         <v>55</v>
@@ -1453,14 +1453,14 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="37" t="s">
         <v>48</v>
       </c>
       <c r="B25" s="38"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
         <v>53</v>
       </c>
@@ -1468,7 +1468,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="21" t="s">
         <v>49</v>
       </c>
@@ -1476,7 +1476,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="21" t="s">
         <v>50</v>
       </c>
@@ -1484,7 +1484,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="21" t="s">
         <v>51</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="22" t="s">
         <v>52</v>
       </c>

</xml_diff>